<commit_message>
theem dataframe cho sheet ketqua
</commit_message>
<xml_diff>
--- a/kpiExcelSheet/nhóm L1.xlsx
+++ b/kpiExcelSheet/nhóm L1.xlsx
@@ -768,7 +768,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1zYsbMX-Gft2b4pZZdDyLumB5I78fhNHAE3t62baPN6s/edit#gid=0
 </t>
@@ -856,7 +856,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://drive.google.com/file/d/1df790NLF5dCua4CjSRZ1jjx1JA3VCXmp/view?usp=drive_link
 </t>
@@ -1003,7 +1003,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1JxytDSIKmv1RNPyIQ0Ocwn1-zJwOdqS4aWsx-ZNBl5o/edit#gid=0
 </t>
@@ -1301,7 +1301,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1RhypsQkAzhg2KbmyNZK4cuOIm6D9OEHNzGXMOfb_1bY/edit?usp=sharing
 </t>
@@ -1518,7 +1518,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1RhypsQkAzhg2KbmyNZK4cuOIm6D9OEHNzGXMOfb_1bY/edit?usp=sharing
 </t>
@@ -1810,7 +1810,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1qUcmCoXKUACHxdPttXY6Avga6qyL18uMcdmXnl0sokM/edit#gid=0
 </t>
@@ -1881,7 +1881,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="8" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
@@ -1898,7 +1898,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">http://172.27.228.249:9000/project/smart-contact-center/issues?tags=lcuat&amp;status=16
 </t>
@@ -2028,7 +2028,7 @@
         <v>103.5</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
@@ -2045,7 +2045,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1cawx0cvzUkyuDyL7H0MyN4sxnIt4dHgQ_njIjm4IFKk/edit#gid=0
 </t>
@@ -2098,7 +2098,7 @@
         <v>197.5</v>
       </c>
       <c r="O24" s="9" t="n">
-        <v>48</v>
+        <v>208</v>
       </c>
       <c r="P24" s="8" t="n">
         <v/>
@@ -2343,7 +2343,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1RhypsQkAzhg2KbmyNZK4cuOIm6D9OEHNzGXMOfb_1bY/edit#gid=994381865
 </t>
@@ -2560,7 +2560,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1RhypsQkAzhg2KbmyNZK4cuOIm6D9OEHNzGXMOfb_1bY/edit#gid=0
 </t>
@@ -2858,7 +2858,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/17eBVsuHjK24RBxa2t94FtApqvEtEebLG04XAQvsHTFA/edit#gid=0
 </t>
@@ -3075,7 +3075,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1WPxs4Ii5gkDtp9GpnjsRl6_j19eP-wKmxDwgii1f5Y4/edit#gid=0
 </t>
@@ -3373,7 +3373,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1zYsbMX-Gft2b4pZZdDyLumB5I78fhNHAE3t62baPN6s/edit#gid=0
 </t>
@@ -3587,7 +3587,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1JxytDSIKmv1RNPyIQ0Ocwn1-zJwOdqS4aWsx-ZNBl5o/edit#gid=0
 </t>
@@ -3952,7 +3952,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/18AWs-XcmlK_jLArRDy4Ylcfo5qZNjfjy/edit#gid=1981640499
 </t>
@@ -3965,7 +3965,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/13xRiQniLrgAGfqB99ZV0Ihw5wJVlOBEs/edit#gid=1187315498
 </t>
@@ -4110,7 +4110,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/13xRiQniLrgAGfqB99ZV0Ihw5wJVlOBEs/edit#gid=167033470
 </t>
@@ -4123,7 +4123,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/13xRiQniLrgAGfqB99ZV0Ihw5wJVlOBEs/edit#gid=167033470
 </t>
@@ -4421,7 +4421,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1szpz8kekeCkkKAiEYem-xqp7zxYnCbDkbBjsgs5UXng/edit#gid=1959940647
 </t>
@@ -4507,7 +4507,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1szpz8kekeCkkKAiEYem-xqp7zxYnCbDkbBjsgs5UXng/edit#gid=1959940647
 </t>
@@ -4651,7 +4651,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1szpz8kekeCkkKAiEYem-xqp7zxYnCbDkbBjsgs5UXng/edit#gid=1959940647
 </t>
@@ -5021,7 +5021,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1_tnT-wl7XPpycFYY5bSZyXZgFFMUZA8BvmnRSb4d8oI/edit?usp=sharing
 </t>
@@ -5170,7 +5170,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/169S8Tj_QKcR8cMRlgrF2b2gnVkYBRcyL/edit?usp=sharing&amp;ouid=111160206982098379432&amp;rtpof=true&amp;sd=true
 </t>
@@ -5468,7 +5468,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1_tnT-wl7XPpycFYY5bSZyXZgFFMUZA8BvmnRSb4d8oI/edit#gid=0
 </t>
@@ -5683,7 +5683,7 @@
           </r>
           <r>
             <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
+              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
             <t xml:space="preserve">https://docs.google.com/spreadsheets/d/169S8Tj_QKcR8cMRlgrF2b2gnVkYBRcyL/edit#gid=1816014955
 </t>

</xml_diff>